<commit_message>
adding login handle to spreadsheet and python file
</commit_message>
<xml_diff>
--- a/UCS.xlsx
+++ b/UCS.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nate/PycharmProjects/UCS-Automation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dad\PycharmProjects\UCS-Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="3440" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2640" yWindow="3435" windowWidth="28800" windowHeight="17595" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,17 +31,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>UCS Workbook for Scripted installation</t>
   </si>
+  <si>
+    <t>IP and Login</t>
+  </si>
+  <si>
+    <t>192.168.1.150</t>
+  </si>
+  <si>
+    <t>IP Address:</t>
+  </si>
+  <si>
+    <t>Username:</t>
+  </si>
+  <si>
+    <t>Password:</t>
+  </si>
+  <si>
+    <t>ucspe</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -69,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -80,6 +107,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -350,11 +380,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -366,13 +398,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.125" customWidth="1"/>
+    <col min="2" max="2" width="17.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -382,7 +451,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -394,7 +463,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -406,7 +475,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Starting to add more information around Chassis Discovery Policy
</commit_message>
<xml_diff>
--- a/UCS.xlsx
+++ b/UCS.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dad\PycharmProjects\UCS-Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nate/PycharmProjects/UCS-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="3435" windowWidth="28800" windowHeight="17595" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2640" yWindow="3440" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="LinkAggregation">Sheet5!$A$1:$A$4</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>UCS Workbook for Scripted installation</t>
   </si>
@@ -53,11 +56,26 @@
   <si>
     <t>ucspe</t>
   </si>
+  <si>
+    <t>Link Aggregation Policy:</t>
+  </si>
+  <si>
+    <t>1-link</t>
+  </si>
+  <si>
+    <t>2-link</t>
+  </si>
+  <si>
+    <t>4-link</t>
+  </si>
+  <si>
+    <t>8-link</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -384,7 +402,7 @@
       <selection activeCell="A4" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -398,16 +416,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B6"/>
+  <dimension ref="A2:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.125" customWidth="1"/>
-    <col min="2" max="2" width="17.75" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -439,7 +457,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+      <formula1>LinkAggregation</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -451,7 +482,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -463,7 +494,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -471,12 +502,35 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>